<commit_message>
updates with new LDA
</commit_message>
<xml_diff>
--- a/data/Sample Log and Raw Data Files/SNL_LDA_figs_UNM.xlsx
+++ b/data/Sample Log and Raw Data Files/SNL_LDA_figs_UNM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexiBesser/Dropbox/Sierra Nevada Lakes AA Isotopes/R Scripts and Associated Analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswall/Desktop/Research and Teaching/github/Sierra-plankton-CSIA/data/Sample Log and Raw Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{48ACC52F-2416-964A-8F5F-1077ECD10FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCA526-FF93-0142-82E8-8403F5780004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1720" windowWidth="32620" windowHeight="19280" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Producers" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,12 @@
     <sheet name="Endmembers LDA" sheetId="3" r:id="rId3"/>
     <sheet name="Zooplankton LDA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
   <si>
     <t>Group</t>
   </si>
@@ -259,16 +256,16 @@
     <t>Elevation</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>y.axis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3467,7 +3464,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0"/>
@@ -3478,10 +3475,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0"/>
+    <sheetView zoomScale="108" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3552,328 +3549,6 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Endmembers"/>
-      <sheetName val="Zooplankton"/>
-      <sheetName val="EndmembersLDA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2">
-            <v>2.6637084169993002</v>
-          </cell>
-          <cell r="D2">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>5.0468807181760402</v>
-          </cell>
-          <cell r="D3">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>2.1431682290209202</v>
-          </cell>
-          <cell r="D4">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>3.7054598166239501</v>
-          </cell>
-          <cell r="D5">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>4.0154537892493796</v>
-          </cell>
-          <cell r="D6">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>2.9852976807304898</v>
-          </cell>
-          <cell r="D7">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>4.2650684125476399</v>
-          </cell>
-          <cell r="D8">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>2.8019214297129298</v>
-          </cell>
-          <cell r="D9">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>2.4839478662222398</v>
-          </cell>
-          <cell r="D10">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>4.1116619615585801</v>
-          </cell>
-          <cell r="D11">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>-5.19625263679134</v>
-          </cell>
-          <cell r="D12">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>-4.7417457669060799</v>
-          </cell>
-          <cell r="D13">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>-3.2492941872036099</v>
-          </cell>
-          <cell r="D14">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>-5.6934235022804103</v>
-          </cell>
-          <cell r="D15">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>-3.5945490140485901</v>
-          </cell>
-          <cell r="D16">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>-5.9398417827096202</v>
-          </cell>
-          <cell r="D17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>-5.80746143090178</v>
-          </cell>
-          <cell r="D18">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="F2">
-            <v>-5.33853130227706</v>
-          </cell>
-          <cell r="G2">
-            <v>1.01</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="F3">
-            <v>1.8762579295080699</v>
-          </cell>
-          <cell r="G3">
-            <v>1.02</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4">
-            <v>0.60788558736406495</v>
-          </cell>
-          <cell r="G4">
-            <v>1.02</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="F5">
-            <v>-4.1754667811928403</v>
-          </cell>
-          <cell r="G5">
-            <v>1.02</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="F6">
-            <v>-4.5346845930594304</v>
-          </cell>
-          <cell r="G6">
-            <v>1.03</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="F7">
-            <v>9.0782251176550297E-2</v>
-          </cell>
-          <cell r="G7">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="F8">
-            <v>-0.42168367353818398</v>
-          </cell>
-          <cell r="G8">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="F9">
-            <v>-4.4021160493613296</v>
-          </cell>
-          <cell r="G9">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="F10">
-            <v>-2.7349715002279198</v>
-          </cell>
-          <cell r="G10">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="F11">
-            <v>0.307240331472521</v>
-          </cell>
-          <cell r="G11">
-            <v>1.05</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="F12">
-            <v>-1.51188236533308</v>
-          </cell>
-          <cell r="G12">
-            <v>1.05</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="F13">
-            <v>-6.9702719217308598E-2</v>
-          </cell>
-          <cell r="G13">
-            <v>1.06</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="F14">
-            <v>-3.0271857844912202</v>
-          </cell>
-          <cell r="G14">
-            <v>1.06</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="F15">
-            <v>-1.9386877473408499</v>
-          </cell>
-          <cell r="G15">
-            <v>1.06</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="F16">
-            <v>-5.16639445608189</v>
-          </cell>
-          <cell r="G16">
-            <v>1.06</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17">
-            <v>-1.59770910974397</v>
-          </cell>
-          <cell r="G17">
-            <v>1.07</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18">
-            <v>-2.8153758237566699</v>
-          </cell>
-          <cell r="G18">
-            <v>1.07</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>-2.9516027816945698</v>
-          </cell>
-          <cell r="G19">
-            <v>1.07</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>-5.7691613792371301</v>
-          </cell>
-          <cell r="G20">
-            <v>1.07</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="F21">
-            <v>-5.2390340218671803</v>
-          </cell>
-          <cell r="G21">
-            <v>1.08</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="F22">
-            <v>-3.9850968540543401</v>
-          </cell>
-          <cell r="G22">
-            <v>1.08</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4172,11 +3847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4196,6 +3871,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4441,11 +4119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4477,6 +4155,9 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -5109,8 +4790,8 @@
       <c r="C29" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>77</v>
+      <c r="D29" s="2">
+        <v>3091</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
@@ -5133,7 +4814,7 @@
         <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -5156,7 +4837,7 @@
         <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -5179,7 +4860,7 @@
         <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
@@ -5202,7 +4883,7 @@
         <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>

</xml_diff>